<commit_message>
Fix Juniper infrastructure costs - remove Professional Services category
- Remove all Professional Services line items from infrastructure-costs.csv
- Professional Services belongs ONLY in level-of-effort-estimate.csv
- Update 3-Year Summary to remove Professional Services row
- SRX Firewall: 3-year total reduced from $539,700 to $438,400 (infrastructure only)
- Mist AI Network: 3-year total reduced from $304,964 to $223,964 (infrastructure only)
- Regenerate all presales documents with corrected infrastructure costs
- Fix Solution Briefing sub-item word counts (<13 words requirement)
</commit_message>
<xml_diff>
--- a/solutions/juniper/cyber-security/srx-firewall-platform/presales/infrastructure-costs.xlsx
+++ b/solutions/juniper/cyber-security/srx-firewall-platform/presales/infrastructure-costs.xlsx
@@ -14,9 +14,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sizing Guidelines'!$A$2:$F$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Infrastructure Costs'!$A$2:$K$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Credits'!$A$2:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3-Year Summary'!$A$2:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Infrastructure Costs'!$A$2:$K$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Credits'!$A$2:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'3-Year Summary'!$A$2:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -836,7 +836,7 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>November 22, 2025</t>
+          <t>November 24, 2025</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1556,7 +1556,7 @@
     <row r="7" ht="26" customHeight="1">
       <c r="A7" s="43" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B7" s="44" t="inlineStr">
@@ -1601,7 +1601,7 @@
     <row r="8" ht="26" customHeight="1">
       <c r="A8" s="47" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B8" s="48" t="inlineStr">
@@ -1646,7 +1646,7 @@
     <row r="9" ht="26" customHeight="1">
       <c r="A9" s="43" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B9" s="44" t="inlineStr">
@@ -1691,7 +1691,7 @@
     <row r="10" ht="26" customHeight="1">
       <c r="A10" s="47" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B10" s="48" t="inlineStr">
@@ -1736,7 +1736,7 @@
     <row r="11" ht="26" customHeight="1">
       <c r="A11" s="43" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B11" s="44" t="inlineStr">
@@ -1781,7 +1781,7 @@
     <row r="12" ht="26" customHeight="1">
       <c r="A12" s="47" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B12" s="48" t="inlineStr">
@@ -1914,441 +1914,36 @@
       </c>
     </row>
     <row r="15" ht="26" customHeight="1">
-      <c r="A15" s="43" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B15" s="44" t="inlineStr">
-        <is>
-          <t>Site Survey and Design</t>
-        </is>
-      </c>
-      <c r="C15" s="44" t="inlineStr">
-        <is>
-          <t>Security architecture design and implementation planning</t>
-        </is>
-      </c>
-      <c r="D15" s="45" t="n">
-        <v>80</v>
-      </c>
-      <c r="E15" s="44" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F15" s="46" t="n">
-        <v>225</v>
-      </c>
-      <c r="G15" s="46" t="n">
-        <v>18000</v>
-      </c>
-      <c r="H15" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="46" t="n">
-        <v>18000</v>
-      </c>
-      <c r="K15" s="44" t="inlineStr">
-        <is>
-          <t>Solution architecture and design</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="26" customHeight="1">
-      <c r="A16" s="47" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B16" s="48" t="inlineStr">
-        <is>
-          <t>Hardware Installation</t>
-        </is>
-      </c>
-      <c r="C16" s="48" t="inlineStr">
-        <is>
-          <t>Rack mount cabling and initial configuration</t>
-        </is>
-      </c>
-      <c r="D16" s="49" t="n">
-        <v>40</v>
-      </c>
-      <c r="E16" s="48" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F16" s="50" t="n">
-        <v>200</v>
-      </c>
-      <c r="G16" s="50" t="n">
-        <v>8000</v>
-      </c>
-      <c r="H16" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="50" t="n">
-        <v>8000</v>
-      </c>
-      <c r="K16" s="48" t="inlineStr">
-        <is>
-          <t>Physical installation services</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="26" customHeight="1">
-      <c r="A17" s="43" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B17" s="44" t="inlineStr">
-        <is>
-          <t>Configuration Services</t>
-        </is>
-      </c>
-      <c r="C17" s="44" t="inlineStr">
-        <is>
-          <t>SRX configuration policy migration and testing</t>
-        </is>
-      </c>
-      <c r="D17" s="45" t="n">
-        <v>120</v>
-      </c>
-      <c r="E17" s="44" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F17" s="46" t="n">
-        <v>225</v>
-      </c>
-      <c r="G17" s="46" t="n">
-        <v>27000</v>
-      </c>
-      <c r="H17" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="46" t="n">
-        <v>27000</v>
-      </c>
-      <c r="K17" s="44" t="inlineStr">
-        <is>
-          <t>Security policy implementation</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="26" customHeight="1">
-      <c r="A18" s="47" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B18" s="48" t="inlineStr">
-        <is>
-          <t>Integration Services</t>
-        </is>
-      </c>
-      <c r="C18" s="48" t="inlineStr">
-        <is>
-          <t>SIEM integration VPN setup and network integration</t>
-        </is>
-      </c>
-      <c r="D18" s="49" t="n">
-        <v>60</v>
-      </c>
-      <c r="E18" s="48" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F18" s="50" t="n">
-        <v>225</v>
-      </c>
-      <c r="G18" s="50" t="n">
-        <v>13500</v>
-      </c>
-      <c r="H18" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="50" t="n">
-        <v>13500</v>
-      </c>
-      <c r="K18" s="48" t="inlineStr">
-        <is>
-          <t>Third-party system integration</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="26" customHeight="1">
-      <c r="A19" s="43" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B19" s="44" t="inlineStr">
-        <is>
-          <t>Testing and Validation</t>
-        </is>
-      </c>
-      <c r="C19" s="44" t="inlineStr">
-        <is>
-          <t>Performance testing security validation and failover testing</t>
-        </is>
-      </c>
-      <c r="D19" s="45" t="n">
-        <v>40</v>
-      </c>
-      <c r="E19" s="44" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F19" s="46" t="n">
-        <v>225</v>
-      </c>
-      <c r="G19" s="46" t="n">
-        <v>9000</v>
-      </c>
-      <c r="H19" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="46" t="n">
-        <v>9000</v>
-      </c>
-      <c r="K19" s="44" t="inlineStr">
-        <is>
-          <t>Pre-production validation</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="26" customHeight="1">
-      <c r="A20" s="47" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B20" s="48" t="inlineStr">
-        <is>
-          <t>Training - Administrator</t>
-        </is>
-      </c>
-      <c r="C20" s="48" t="inlineStr">
-        <is>
-          <t>SRX administration and Junos OS training (2 days)</t>
-        </is>
-      </c>
-      <c r="D20" s="49" t="n">
-        <v>16</v>
-      </c>
-      <c r="E20" s="48" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F20" s="50" t="n">
-        <v>200</v>
-      </c>
-      <c r="G20" s="50" t="n">
-        <v>3200</v>
-      </c>
-      <c r="H20" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="50" t="n">
-        <v>3200</v>
-      </c>
-      <c r="K20" s="48" t="inlineStr">
-        <is>
-          <t>Technical team enablement</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="26" customHeight="1">
-      <c r="A21" s="43" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B21" s="44" t="inlineStr">
-        <is>
-          <t>Training - Security Operations</t>
-        </is>
-      </c>
-      <c r="C21" s="44" t="inlineStr">
-        <is>
-          <t>Security policy management and operations training (1 day)</t>
-        </is>
-      </c>
-      <c r="D21" s="45" t="n">
-        <v>8</v>
-      </c>
-      <c r="E21" s="44" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F21" s="46" t="n">
-        <v>200</v>
-      </c>
-      <c r="G21" s="46" t="n">
-        <v>1600</v>
-      </c>
-      <c r="H21" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="46" t="n">
-        <v>1600</v>
-      </c>
-      <c r="K21" s="44" t="inlineStr">
-        <is>
-          <t>SOC team training</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="26" customHeight="1">
-      <c r="A22" s="47" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B22" s="48" t="inlineStr">
-        <is>
-          <t>Deployment Support</t>
-        </is>
-      </c>
-      <c r="C22" s="48" t="inlineStr">
-        <is>
-          <t>On-site go-live support and knowledge transfer</t>
-        </is>
-      </c>
-      <c r="D22" s="49" t="n">
-        <v>40</v>
-      </c>
-      <c r="E22" s="48" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F22" s="50" t="n">
-        <v>225</v>
-      </c>
-      <c r="G22" s="50" t="n">
-        <v>9000</v>
-      </c>
-      <c r="H22" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="50" t="n">
-        <v>9000</v>
-      </c>
-      <c r="K22" s="48" t="inlineStr">
-        <is>
-          <t>Deployment assistance</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="26" customHeight="1">
-      <c r="A23" s="43" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B23" s="44" t="inlineStr">
-        <is>
-          <t>Project Management</t>
-        </is>
-      </c>
-      <c r="C23" s="44" t="inlineStr">
-        <is>
-          <t>Project coordination and stakeholder management</t>
-        </is>
-      </c>
-      <c r="D23" s="45" t="n">
-        <v>80</v>
-      </c>
-      <c r="E23" s="44" t="inlineStr">
-        <is>
-          <t>Hours</t>
-        </is>
-      </c>
-      <c r="F23" s="46" t="n">
-        <v>150</v>
-      </c>
-      <c r="G23" s="46" t="n">
-        <v>12000</v>
-      </c>
-      <c r="H23" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="46" t="n">
-        <v>12000</v>
-      </c>
-      <c r="K23" s="44" t="inlineStr">
-        <is>
-          <t>Overall project delivery</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="26" customHeight="1">
-      <c r="A24" s="51" t="inlineStr">
+      <c r="A15" s="51" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B24" s="52" t="n"/>
-      <c r="C24" s="52" t="n"/>
-      <c r="D24" s="52" t="n"/>
-      <c r="E24" s="52" t="n"/>
-      <c r="F24" s="52" t="n"/>
-      <c r="G24" s="53">
-        <f>SUM(G3:G23)</f>
-        <v/>
-      </c>
-      <c r="H24" s="53">
-        <f>SUM(H3:H23)</f>
-        <v/>
-      </c>
-      <c r="I24" s="53">
-        <f>SUM(I3:I23)</f>
-        <v/>
-      </c>
-      <c r="J24" s="53">
-        <f>SUM(J3:J23)</f>
-        <v/>
-      </c>
-      <c r="K24" s="52" t="n"/>
+      <c r="B15" s="52" t="n"/>
+      <c r="C15" s="52" t="n"/>
+      <c r="D15" s="52" t="n"/>
+      <c r="E15" s="52" t="n"/>
+      <c r="F15" s="52" t="n"/>
+      <c r="G15" s="53">
+        <f>SUM(G3:G14)</f>
+        <v/>
+      </c>
+      <c r="H15" s="53">
+        <f>SUM(H3:H14)</f>
+        <v/>
+      </c>
+      <c r="I15" s="53">
+        <f>SUM(I3:I14)</f>
+        <v/>
+      </c>
+      <c r="J15" s="53">
+        <f>SUM(J3:J14)</f>
+        <v/>
+      </c>
+      <c r="K15" s="52" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K24"/>
+  <autoFilter ref="A2:K15"/>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
@@ -2362,7 +1957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -2429,7 +2024,7 @@
     <row r="4" ht="26" customHeight="1">
       <c r="A4" s="47" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B4" s="48" t="inlineStr">
@@ -2466,28 +2061,8 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="26" customHeight="1">
-      <c r="A6" s="47" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B6" s="48" t="inlineStr">
-        <is>
-          <t>Partner Credit</t>
-        </is>
-      </c>
-      <c r="C6" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="48" t="inlineStr">
-        <is>
-          <t>No professional services credits available</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:D6"/>
+  <autoFilter ref="A2:D5"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -2501,7 +2076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -2597,7 +2172,7 @@
     <row r="4" ht="26" customHeight="1">
       <c r="A4" s="47" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Software Licenses</t>
         </is>
       </c>
       <c r="B4" s="50">
@@ -2657,69 +2232,38 @@
       </c>
     </row>
     <row r="6" ht="26" customHeight="1">
-      <c r="A6" s="47" t="inlineStr">
-        <is>
-          <t>Professional Services</t>
-        </is>
-      </c>
-      <c r="B6" s="50">
-        <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$G:$G)</f>
-        <v/>
-      </c>
-      <c r="C6" s="50">
-        <f>SUMIF(Credits!$A:$A,A6,Credits!$C:$C)</f>
-        <v/>
-      </c>
-      <c r="D6" s="50">
-        <f>B6+C6</f>
-        <v/>
-      </c>
-      <c r="E6" s="50">
-        <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$H:$H)</f>
-        <v/>
-      </c>
-      <c r="F6" s="50">
-        <f>SUMIF('Infrastructure Costs'!$A:$A,A6,'Infrastructure Costs'!$I:$I)</f>
-        <v/>
-      </c>
-      <c r="G6" s="50">
-        <f>D6+E6+F6</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" ht="26" customHeight="1">
-      <c r="A7" s="51" t="inlineStr">
+      <c r="A6" s="51" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B7" s="53">
-        <f>SUM(B3:B6)</f>
-        <v/>
-      </c>
-      <c r="C7" s="53">
-        <f>SUM(C3:C6)</f>
-        <v/>
-      </c>
-      <c r="D7" s="53">
-        <f>SUM(D3:D6)</f>
-        <v/>
-      </c>
-      <c r="E7" s="53">
-        <f>SUM(E3:E6)</f>
-        <v/>
-      </c>
-      <c r="F7" s="53">
-        <f>SUM(F3:F6)</f>
-        <v/>
-      </c>
-      <c r="G7" s="53">
-        <f>SUM(G3:G6)</f>
+      <c r="B6" s="53">
+        <f>SUM(B3:B5)</f>
+        <v/>
+      </c>
+      <c r="C6" s="53">
+        <f>SUM(C3:C5)</f>
+        <v/>
+      </c>
+      <c r="D6" s="53">
+        <f>SUM(D3:D5)</f>
+        <v/>
+      </c>
+      <c r="E6" s="53">
+        <f>SUM(E3:E5)</f>
+        <v/>
+      </c>
+      <c r="F6" s="53">
+        <f>SUM(F3:F5)</f>
+        <v/>
+      </c>
+      <c r="G6" s="53">
+        <f>SUM(G3:G5)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G7"/>
+  <autoFilter ref="A2:G6"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>